<commit_message>
change units , order inputs ,
TODO: api from pvgis not working
</commit_message>
<xml_diff>
--- a/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
+++ b/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Hotmaps\dispatch_module\cm\app\api_v1\my_calculation_module_directory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Hotmaps\dispatch_module\cm\app\api_v1\my_calculation_module_directory\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FEDD0F-D261-49F5-92BF-CEB0BB301155}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FFDDCA-700E-4F3D-B184-43EEE99E1DD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{A39C18F9-790E-4AC0-B0AE-6D70F2BE89C8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="130">
   <si>
     <t>input_name</t>
   </si>
@@ -168,9 +168,6 @@
     <t>wi_opexVar</t>
   </si>
   <si>
-    <t>electricity_p</t>
-  </si>
-  <si>
     <t>waste_p</t>
   </si>
   <si>
@@ -264,15 +261,6 @@
     <t xml:space="preserve">energy carrier price - Bio Gas </t>
   </si>
   <si>
-    <t>invest mode-</t>
-  </si>
-  <si>
-    <t>interest rate -</t>
-  </si>
-  <si>
-    <t>CO2 Price -</t>
-  </si>
-  <si>
     <t xml:space="preserve">energy carrier price - various </t>
   </si>
   <si>
@@ -282,15 +270,9 @@
     <t xml:space="preserve">electrical efficiency -Back Pressure CHP </t>
   </si>
   <si>
-    <t xml:space="preserve"> Thermal Output Capacity  -Back Pressure CHP </t>
-  </si>
-  <si>
     <t xml:space="preserve">energy carrier -Back Pressure CHP </t>
   </si>
   <si>
-    <t xml:space="preserve"> investment cost -Back Pressure CHP </t>
-  </si>
-  <si>
     <t xml:space="preserve">lifetime -Back Pressure CHP </t>
   </si>
   <si>
@@ -309,9 +291,6 @@
     <t xml:space="preserve">electrical efficiency -Solar Thermal </t>
   </si>
   <si>
-    <t xml:space="preserve">energy carrier price -electricity </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Thermal Output Capacity -Heat Boiler </t>
   </si>
   <si>
@@ -396,9 +375,6 @@
     <t xml:space="preserve">thermal efficiency -Heat Boiler </t>
   </si>
   <si>
-    <t xml:space="preserve"> Thermal Output Capacity -Waste Incineration Plant </t>
-  </si>
-  <si>
     <t>energy carrier -Waste Incineration Plant</t>
   </si>
   <si>
@@ -408,9 +384,6 @@
     <t>lifetime -Waste Incineration Plant</t>
   </si>
   <si>
-    <t>thermal efficiency -Heat Pump</t>
-  </si>
-  <si>
     <t xml:space="preserve">thermal efficiency -Solar Thermal </t>
   </si>
   <si>
@@ -424,6 +397,27 @@
   </si>
   <si>
     <t xml:space="preserve">energy carrier price -wood pellets </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Output Capacity  -Back Pressure CHP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">investment cost -Back Pressure CHP </t>
+  </si>
+  <si>
+    <t>invest mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interest rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2 Price </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Output Capacity -Waste Incineration Plant </t>
+  </si>
+  <si>
+    <t>COP -Heat Pump</t>
   </si>
 </sst>
 </file>
@@ -473,12 +467,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -793,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED82753-5272-4518-B7D2-E7729D132D1F}">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,8 +802,9 @@
     <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -840,64 +836,68 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
-        <v>1</v>
+      <c r="H2" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -908,93 +908,103 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>75</v>
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="4">
-        <v>800000</v>
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="D7">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1">
@@ -1004,90 +1014,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
+        <v>125</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="4">
-        <v>46000</v>
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>0.6</v>
       </c>
       <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D11">
-        <v>4.5</v>
+        <v>0.875</v>
       </c>
       <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1102,134 +1107,136 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D13">
-        <v>60</v>
+        <v>0.6</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="1">
         <v>0</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>0.2</v>
       </c>
       <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="4">
-        <v>60000</v>
+        <v>58</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="F16" t="s">
-        <v>21</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="1">
         <v>0</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="D17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>3</v>
-      </c>
-      <c r="F17" t="s">
-        <v>23</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D18">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1244,27 +1251,27 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D19">
-        <v>0.20200000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
-        <v>34</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1">
         <v>0</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1274,336 +1281,300 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="4">
-        <v>4000</v>
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D21">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="D22">
-        <v>20</v>
+        <v>0.114</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" t="s">
         <v>70</v>
       </c>
+      <c r="D23">
+        <v>0.312</v>
+      </c>
       <c r="E23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="4">
-        <v>750000</v>
+        <v>71</v>
+      </c>
+      <c r="D24">
+        <v>0.20200000000000001</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="1">
-        <v>0</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D25">
-        <v>25</v>
+        <v>0.09</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26">
-        <v>0.09</v>
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
       </c>
       <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="1">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
       </c>
       <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="1">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="4">
-        <v>34000</v>
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
       </c>
       <c r="E28">
-        <v>3</v>
-      </c>
-      <c r="F28" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="1">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29">
-        <v>0.5</v>
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>73</v>
       </c>
       <c r="E29">
-        <v>3</v>
-      </c>
-      <c r="F29" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="1">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" t="s">
         <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D31">
-        <v>7.0000000000000007E-2</v>
+        <v>40</v>
       </c>
       <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1">
-        <v>0</v>
-      </c>
-      <c r="H31" s="1">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D32">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
-      </c>
-      <c r="G32" s="1">
-        <v>0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" s="1">
-        <v>0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1614,69 +1585,69 @@
       <c r="F34" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
+      <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D35">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="1">
-        <v>0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" t="s">
-        <v>74</v>
+        <v>32</v>
+      </c>
+      <c r="D36" s="4">
+        <v>800000</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37">
-        <v>1030000</v>
+        <v>29</v>
+      </c>
+      <c r="D37" s="4">
+        <v>60000</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -1687,282 +1658,308 @@
       <c r="G37" s="1">
         <v>0</v>
       </c>
-      <c r="H37" s="1"/>
+      <c r="H37" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="D38" s="4">
+        <v>750000</v>
       </c>
       <c r="E38">
         <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G38" s="1">
         <v>0</v>
       </c>
-      <c r="H38" s="1"/>
+      <c r="H38" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="D39">
-        <v>0.114</v>
+        <v>1030000</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G39" s="1">
         <v>0</v>
       </c>
-      <c r="H39" s="1"/>
+      <c r="H39" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40">
-        <v>0.312</v>
+        <v>33</v>
+      </c>
+      <c r="D40" s="4">
+        <v>3200000</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F40" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G40" s="1">
         <v>0</v>
       </c>
-      <c r="H40" s="1"/>
+      <c r="H40" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D41" s="4">
-        <v>30000</v>
+        <v>27</v>
+      </c>
+      <c r="D41">
+        <v>25</v>
       </c>
       <c r="E41">
         <v>3</v>
       </c>
       <c r="F41" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G41" s="1">
         <v>0</v>
       </c>
-      <c r="H41" s="1"/>
+      <c r="H41" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D42">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="E42">
         <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G42" s="1">
         <v>0</v>
       </c>
-      <c r="H42" s="1"/>
+      <c r="H42" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="D43">
-        <v>0.6</v>
+        <v>25</v>
       </c>
       <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>23</v>
+      </c>
       <c r="G43" s="1">
         <v>0</v>
       </c>
       <c r="H43" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D44">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E44">
         <v>3</v>
       </c>
       <c r="F44" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G44" s="1">
         <v>0</v>
       </c>
-      <c r="H44" s="1"/>
+      <c r="H44" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D45">
-        <v>0.875</v>
+        <v>25</v>
       </c>
       <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F45" t="s">
+        <v>23</v>
+      </c>
       <c r="G45" s="1">
         <v>0</v>
       </c>
       <c r="H45" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
-      </c>
-      <c r="D46">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="D46" s="4">
+        <v>46000</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G46" s="1">
         <v>0</v>
       </c>
-      <c r="H46" s="1"/>
+      <c r="H46" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="D47" s="4">
+        <v>4000</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F47" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
       </c>
-      <c r="H47" s="1"/>
+      <c r="H47" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" t="s">
-        <v>76</v>
+        <v>37</v>
+      </c>
+      <c r="D48" s="4">
+        <v>34000</v>
       </c>
       <c r="E48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F48" t="s">
-        <v>22</v>
-      </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D49" s="4">
-        <v>3200000</v>
+        <v>30000</v>
       </c>
       <c r="E49">
         <v>3</v>
@@ -1973,113 +1970,123 @@
       <c r="G49" s="1">
         <v>0</v>
       </c>
-      <c r="H49" s="1"/>
+      <c r="H49" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>28</v>
-      </c>
-      <c r="D50">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="D50" s="4">
+        <v>90000</v>
       </c>
       <c r="E50">
         <v>3</v>
       </c>
       <c r="F50" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G50" s="1">
         <v>0</v>
       </c>
-      <c r="H50" s="1"/>
+      <c r="H50" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D51">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F51" t="s">
+        <v>22</v>
+      </c>
       <c r="G51" s="1">
         <v>0</v>
       </c>
-      <c r="H51" s="1">
-        <v>1</v>
+      <c r="H51" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F52" t="s">
+        <v>22</v>
+      </c>
       <c r="G52" s="1">
         <v>0</v>
       </c>
-      <c r="H52" s="1">
-        <v>1</v>
+      <c r="H52" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" s="4">
-        <v>90000</v>
+        <v>42</v>
+      </c>
+      <c r="D53">
+        <v>0.5</v>
       </c>
       <c r="E53">
         <v>3</v>
       </c>
       <c r="F53" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G53" s="1">
         <v>0</v>
       </c>
-      <c r="H53" s="1"/>
+      <c r="H53" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D54">
         <v>0.5</v>
@@ -2093,61 +2100,44 @@
       <c r="G54" s="1">
         <v>0</v>
       </c>
-      <c r="H54" s="1"/>
+      <c r="H54" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D55">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E55">
-        <v>1</v>
-      </c>
-      <c r="F55" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F55" t="s">
+        <v>22</v>
+      </c>
       <c r="G55" s="1">
         <v>0</v>
       </c>
-      <c r="H55" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>131</v>
-      </c>
-      <c r="B56" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" t="s">
-        <v>68</v>
-      </c>
-      <c r="D56">
-        <v>44</v>
-      </c>
-      <c r="E56">
-        <v>3</v>
-      </c>
-      <c r="F56" t="s">
-        <v>22</v>
-      </c>
-      <c r="G56" s="1">
-        <v>0</v>
-      </c>
-      <c r="H56" s="1"/>
+      <c r="H55" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I62" s="1"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I64" s="1"/>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I66" s="1"/>
     </row>
     <row r="67" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I67" s="1"/>
@@ -2161,11 +2151,12 @@
     <row r="70" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I71" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H56" xr:uid="{5C6FFFE4-1DCD-43ED-AC49-CFF8C14D347B}"/>
+  <autoFilter ref="A1:H55" xr:uid="{5C6FFFE4-1DCD-43ED-AC49-CFF8C14D347B}">
+    <sortState ref="A2:H55">
+      <sortCondition ref="E1:E55"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
bug fixi rename some indicators
</commit_message>
<xml_diff>
--- a/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
+++ b/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Hotmaps\dispatch_module\cm\app\api_v1\my_calculation_module_directory\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FFDDCA-700E-4F3D-B184-43EEE99E1DD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A865E10-37E8-4526-B41A-4C7045FB5615}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{A39C18F9-790E-4AC0-B0AE-6D70F2BE89C8}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="131">
   <si>
     <t>input_name</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>COP -Heat Pump</t>
+  </si>
+  <si>
+    <t>EUR/(MW*yr)</t>
   </si>
 </sst>
 </file>
@@ -791,7 +794,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +848,7 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>1E-3</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -871,7 +874,7 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>30</v>
+        <v>1E-3</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -897,7 +900,7 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>1E-3</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -923,7 +926,7 @@
         <v>13</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <v>1E-3</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -949,7 +952,7 @@
         <v>14</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>1E-3</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1292,8 +1295,12 @@
       <c r="F20" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="G20" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H20" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1314,8 +1321,12 @@
       <c r="F21" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="G21" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H21" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1336,8 +1347,12 @@
       <c r="F22" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="G22" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H22" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1358,8 +1373,12 @@
       <c r="F23" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="G23" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H23" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1380,8 +1399,12 @@
       <c r="F24" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="G24" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H24" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1402,8 +1425,12 @@
       <c r="F25" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="G25" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H25" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1519,8 +1546,12 @@
       <c r="F31" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="G31" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H31" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1541,8 +1572,12 @@
       <c r="F32" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="G32" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H32" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1563,8 +1598,12 @@
       <c r="F33" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="G33" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H33" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1585,8 +1624,12 @@
       <c r="F34" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="G34" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H34" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1607,8 +1650,12 @@
       <c r="F35" t="s">
         <v>22</v>
       </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="G35" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H35" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1887,7 +1934,7 @@
         <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="G46" s="1">
         <v>0</v>
@@ -1913,7 +1960,7 @@
         <v>3</v>
       </c>
       <c r="F47" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
@@ -1939,7 +1986,7 @@
         <v>3</v>
       </c>
       <c r="F48" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
@@ -1965,7 +2012,7 @@
         <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="G49" s="1">
         <v>0</v>
@@ -1991,7 +2038,7 @@
         <v>3</v>
       </c>
       <c r="F50" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="G50" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
reorder inputs add 2 extra inputs
</commit_message>
<xml_diff>
--- a/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
+++ b/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Hotmaps\dispatch_module\cm\app\api_v1\my_calculation_module_directory\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A454199-FDEB-4313-AAD9-FCA4EF8D30D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09956563-8E01-4C90-922F-9C62CF728788}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{A39C18F9-790E-4AC0-B0AE-6D70F2BE89C8}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="177">
   <si>
     <t>input_name</t>
   </si>
@@ -291,9 +291,6 @@
     <t xml:space="preserve">electrical efficiency -Solar Thermal </t>
   </si>
   <si>
-    <t xml:space="preserve"> Thermal Output Capacity -Heat Boiler </t>
-  </si>
-  <si>
     <t xml:space="preserve">energy carrier -Heat Boiler </t>
   </si>
   <si>
@@ -315,9 +312,6 @@
     <t xml:space="preserve">OPEX var -Heat Boiler </t>
   </si>
   <si>
-    <t xml:space="preserve"> Thermal Output Capacity  -Heat Pump </t>
-  </si>
-  <si>
     <t xml:space="preserve">energy carrier -Heat Pump  </t>
   </si>
   <si>
@@ -345,9 +339,6 @@
     <t>energy carrier price -radiation</t>
   </si>
   <si>
-    <t xml:space="preserve"> Thermal Output Capacity  -Solar Thermal </t>
-  </si>
-  <si>
     <t xml:space="preserve">energy carrier -Solar Thermal </t>
   </si>
   <si>
@@ -544,6 +535,30 @@
   </si>
   <si>
     <t xml:space="preserve">fix sale electricity price -Heat Boiler </t>
+  </si>
+  <si>
+    <t xml:space="preserve">input </t>
+  </si>
+  <si>
+    <t>chp_ramp</t>
+  </si>
+  <si>
+    <t>ramping cost  -Back Pressure CHP</t>
+  </si>
+  <si>
+    <t>ramping cost  -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Output Capacity  -Solar Thermal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Output Capacity  -Heat Pump </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Output Capacity -Heat Boiler </t>
+  </si>
+  <si>
+    <t>wi_ramp</t>
   </si>
 </sst>
 </file>
@@ -914,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED82753-5272-4518-B7D2-E7729D132D1F}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,13 +977,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -988,13 +1003,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1014,13 +1029,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1040,13 +1055,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1066,7 +1081,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -1092,7 +1107,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1118,7 +1133,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1142,7 +1157,7 @@
     </row>
     <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>20</v>
@@ -1161,7 +1176,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -1185,16 +1200,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D11">
-        <v>0.875</v>
+        <v>0.2</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1209,71 +1224,63 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
+        <v>135</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13">
-        <v>0.6</v>
+        <v>136</v>
+      </c>
+      <c r="D13" t="s">
+        <v>132</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1">
-        <v>0</v>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="5">
+        <v>-9.9999999999999998E+101</v>
       </c>
       <c r="H14" s="5">
         <v>9.9999999999999998E+101</v>
@@ -1281,40 +1288,42 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D15">
-        <v>0.2</v>
+        <v>0.09</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>1</v>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H15" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1329,13 +1338,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1353,16 +1362,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1371,22 +1380,22 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="H18" s="1">
-        <v>1</v>
+      <c r="H18" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D19">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1401,7 +1410,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1427,68 +1436,64 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H21" s="5">
-        <v>9.9999999999999998E+101</v>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D22">
-        <v>0.114</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H22" s="5">
-        <v>9.9999999999999998E+101</v>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D23">
-        <v>0.312</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1505,16 +1510,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D24">
-        <v>0.20200000000000001</v>
+        <v>0.114</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1531,140 +1536,157 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D25">
-        <v>0.09</v>
+        <v>0.6</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H25" s="5">
-        <v>9.9999999999999998E+101</v>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" t="s">
-        <v>74</v>
+        <v>62</v>
+      </c>
+      <c r="D26">
+        <v>0.15</v>
       </c>
       <c r="E26">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="D29">
+        <v>0.312</v>
       </c>
       <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H29" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="D30">
+        <v>40</v>
       </c>
       <c r="E30">
         <v>2</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H30" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D31">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
         <v>22</v>
@@ -1678,19 +1700,19 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D32">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="s">
         <v>22</v>
@@ -1704,19 +1726,19 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="s">
         <v>22</v>
@@ -1730,19 +1752,19 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="s">
         <v>22</v>
@@ -1756,16 +1778,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>170</v>
       </c>
       <c r="D35">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -1782,42 +1804,35 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="4">
-        <v>800000</v>
+        <v>18</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
       </c>
       <c r="E36">
         <v>3</v>
       </c>
-      <c r="F36" t="s">
-        <v>21</v>
-      </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D37" s="4">
-        <v>60000</v>
+        <v>800000</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -1834,48 +1849,48 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" s="4">
-        <v>750000</v>
+        <v>27</v>
+      </c>
+      <c r="D38">
+        <v>25</v>
       </c>
       <c r="E38">
         <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G38" s="1">
         <v>0</v>
       </c>
-      <c r="H38" s="5">
-        <v>9.9999999999999998E+101</v>
+      <c r="H38" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39">
-        <v>1030000</v>
+        <v>39</v>
+      </c>
+      <c r="D39" s="4">
+        <v>46000</v>
       </c>
       <c r="E39">
         <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="G39" s="1">
         <v>0</v>
@@ -1886,22 +1901,22 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="4">
-        <v>3200000</v>
+        <v>44</v>
+      </c>
+      <c r="D40">
+        <v>4.5</v>
       </c>
       <c r="E40">
         <v>3</v>
       </c>
       <c r="F40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G40" s="1">
         <v>0</v>
@@ -1912,120 +1927,113 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="D41">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E41">
         <v>3</v>
       </c>
       <c r="F41" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="1">
-        <v>0</v>
-      </c>
-      <c r="H41" s="1">
-        <v>100</v>
+        <v>22</v>
+      </c>
+      <c r="G41" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H41" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="D42">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E42">
         <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>23</v>
-      </c>
-      <c r="G42" s="1">
-        <v>0</v>
-      </c>
-      <c r="H42" s="1">
-        <v>100</v>
+        <v>22</v>
+      </c>
+      <c r="G42" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H42" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
+        <v>72</v>
       </c>
       <c r="E43">
         <v>3</v>
       </c>
-      <c r="F43" t="s">
-        <v>23</v>
-      </c>
-      <c r="G43" s="1">
-        <v>0</v>
-      </c>
-      <c r="H43" s="1">
-        <v>100</v>
-      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>26</v>
-      </c>
-      <c r="D44">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="D44" s="4">
+        <v>60000</v>
       </c>
       <c r="E44">
         <v>3</v>
       </c>
       <c r="F44" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G44" s="1">
         <v>0</v>
       </c>
-      <c r="H44" s="1">
-        <v>100</v>
+      <c r="H44" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D45">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E45">
         <v>3</v>
@@ -2042,22 +2050,22 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D46" s="4">
-        <v>46000</v>
+        <v>4000</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G46" s="1">
         <v>0</v>
@@ -2074,16 +2082,16 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" s="4">
-        <v>4000</v>
+        <v>41</v>
+      </c>
+      <c r="D47">
+        <v>1.5</v>
       </c>
       <c r="E47">
         <v>3</v>
       </c>
       <c r="F47" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
@@ -2094,77 +2102,59 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
-      </c>
-      <c r="D48" s="4">
-        <v>34000</v>
+        <v>155</v>
+      </c>
+      <c r="D48" t="s">
+        <v>132</v>
       </c>
       <c r="E48">
         <v>3</v>
-      </c>
-      <c r="F48" t="s">
-        <v>130</v>
-      </c>
-      <c r="G48" s="1">
-        <v>0</v>
-      </c>
-      <c r="H48" s="5">
-        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
-      </c>
-      <c r="D49" s="4">
-        <v>30000</v>
+        <v>150</v>
+      </c>
+      <c r="D49" t="s">
+        <v>132</v>
       </c>
       <c r="E49">
         <v>3</v>
-      </c>
-      <c r="F49" t="s">
-        <v>130</v>
-      </c>
-      <c r="G49" s="1">
-        <v>0</v>
-      </c>
-      <c r="H49" s="5">
-        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="4">
-        <v>90000</v>
+        <v>163</v>
+      </c>
+      <c r="D50">
+        <v>45</v>
       </c>
       <c r="E50">
         <v>3</v>
       </c>
       <c r="F50" t="s">
-        <v>130</v>
-      </c>
-      <c r="G50" s="1">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="G50" s="5">
+        <v>-9.9999999999999998E+101</v>
       </c>
       <c r="H50" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2172,16 +2162,16 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="D51">
-        <v>4.5</v>
+        <v>45</v>
       </c>
       <c r="E51">
         <v>3</v>
@@ -2189,8 +2179,8 @@
       <c r="F51" t="s">
         <v>22</v>
       </c>
-      <c r="G51" s="1">
-        <v>0</v>
+      <c r="G51" s="5">
+        <v>-9.9999999999999998E+101</v>
       </c>
       <c r="H51" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2198,68 +2188,50 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D52">
-        <v>1.5</v>
+        <v>148</v>
+      </c>
+      <c r="D52" t="s">
+        <v>132</v>
       </c>
       <c r="E52">
         <v>3</v>
-      </c>
-      <c r="F52" t="s">
-        <v>22</v>
-      </c>
-      <c r="G52" s="1">
-        <v>0</v>
-      </c>
-      <c r="H52" s="5">
-        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C53" t="s">
-        <v>42</v>
-      </c>
-      <c r="D53">
-        <v>0.5</v>
+        <v>157</v>
+      </c>
+      <c r="D53" t="s">
+        <v>132</v>
       </c>
       <c r="E53">
         <v>3</v>
-      </c>
-      <c r="F53" t="s">
-        <v>22</v>
-      </c>
-      <c r="G53" s="1">
-        <v>0</v>
-      </c>
-      <c r="H53" s="5">
-        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>151</v>
       </c>
       <c r="D54">
-        <v>0.5</v>
+        <v>45</v>
       </c>
       <c r="E54">
         <v>3</v>
@@ -2267,8 +2239,8 @@
       <c r="F54" t="s">
         <v>22</v>
       </c>
-      <c r="G54" s="1">
-        <v>0</v>
+      <c r="G54" s="5">
+        <v>-9.9999999999999998E+101</v>
       </c>
       <c r="H54" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2276,16 +2248,16 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
       </c>
       <c r="C55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D55">
         <v>45</v>
-      </c>
-      <c r="D55">
-        <v>0.5</v>
       </c>
       <c r="E55">
         <v>3</v>
@@ -2293,8 +2265,8 @@
       <c r="F55" t="s">
         <v>22</v>
       </c>
-      <c r="G55" s="1">
-        <v>0</v>
+      <c r="G55" s="5">
+        <v>-9.9999999999999998E+101</v>
       </c>
       <c r="H55" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2302,92 +2274,113 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="B56" t="s">
         <v>20</v>
       </c>
       <c r="C56" t="s">
-        <v>143</v>
+        <v>16</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
+        <v>69</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
-      </c>
-      <c r="D57" t="s">
-        <v>135</v>
+        <v>30</v>
+      </c>
+      <c r="D57" s="4">
+        <v>750000</v>
       </c>
       <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F57" t="s">
+        <v>21</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>144</v>
-      </c>
-      <c r="D58" t="s">
-        <v>135</v>
+        <v>25</v>
+      </c>
+      <c r="D58">
+        <v>25</v>
       </c>
       <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>139</v>
-      </c>
-      <c r="D59" t="s">
-        <v>135</v>
+        <v>37</v>
+      </c>
+      <c r="D59" s="4">
+        <v>34000</v>
       </c>
       <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F59" t="s">
+        <v>127</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>42</v>
       </c>
       <c r="D60">
-        <v>45</v>
+        <v>0.5</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -2395,8 +2388,8 @@
       <c r="F60" t="s">
         <v>22</v>
       </c>
-      <c r="G60" s="5">
-        <v>-9.9999999999999998E+101</v>
+      <c r="G60" s="1">
+        <v>0</v>
       </c>
       <c r="H60" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2404,51 +2397,44 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="B61" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C61" t="s">
-        <v>136</v>
-      </c>
-      <c r="D61">
-        <v>45</v>
+        <v>17</v>
+      </c>
+      <c r="D61" t="s">
+        <v>73</v>
       </c>
       <c r="E61">
         <v>3</v>
       </c>
-      <c r="F61" t="s">
-        <v>22</v>
-      </c>
-      <c r="G61" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H61" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
       <c r="D62">
-        <v>45</v>
+        <v>1030000</v>
       </c>
       <c r="E62">
         <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>22</v>
-      </c>
-      <c r="G62" s="5">
-        <v>-9.9999999999999998E+101</v>
+        <v>21</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
       </c>
       <c r="H62" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2457,79 +2443,97 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>137</v>
+        <v>26</v>
       </c>
       <c r="D63">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E63">
         <v>3</v>
       </c>
       <c r="F63" t="s">
-        <v>22</v>
-      </c>
-      <c r="G63" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H63" s="5">
-        <v>9.9999999999999998E+101</v>
+        <v>23</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>100</v>
       </c>
       <c r="I63" s="1"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="B64" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>151</v>
-      </c>
-      <c r="D64" t="s">
-        <v>135</v>
+        <v>38</v>
+      </c>
+      <c r="D64" s="4">
+        <v>30000</v>
       </c>
       <c r="E64">
         <v>3</v>
+      </c>
+      <c r="F64" t="s">
+        <v>127</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
       <c r="I64" s="1"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>152</v>
-      </c>
-      <c r="D65" t="s">
-        <v>135</v>
+        <v>43</v>
+      </c>
+      <c r="D65">
+        <v>0.5</v>
       </c>
       <c r="E65">
         <v>3</v>
+      </c>
+      <c r="F65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
+      <c r="H65" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
       <c r="I65" s="1"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B66" t="s">
         <v>20</v>
       </c>
       <c r="C66" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D66" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E66">
         <v>3</v>
@@ -2538,16 +2542,16 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B67" t="s">
         <v>20</v>
       </c>
       <c r="C67" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D67" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E67">
         <v>3</v>
@@ -2559,84 +2563,95 @@
         <v>161</v>
       </c>
       <c r="B68" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>162</v>
-      </c>
-      <c r="D68" t="s">
-        <v>135</v>
+        <v>152</v>
+      </c>
+      <c r="D68">
+        <v>45</v>
       </c>
       <c r="E68">
         <v>3</v>
+      </c>
+      <c r="F68" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H68" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
       <c r="I68" s="1"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="B69" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>153</v>
-      </c>
-      <c r="D69" t="s">
-        <v>135</v>
+        <v>167</v>
+      </c>
+      <c r="D69">
+        <v>45</v>
       </c>
       <c r="E69">
         <v>3</v>
+      </c>
+      <c r="F69" t="s">
+        <v>22</v>
+      </c>
+      <c r="G69" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H69" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
       <c r="I69" s="1"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C70" t="s">
-        <v>154</v>
-      </c>
-      <c r="D70">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="D70" t="s">
+        <v>75</v>
       </c>
       <c r="E70">
         <v>3</v>
       </c>
-      <c r="F70" t="s">
-        <v>22</v>
-      </c>
-      <c r="G70" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H70" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>155</v>
-      </c>
-      <c r="D71">
-        <v>45</v>
+        <v>33</v>
+      </c>
+      <c r="D71" s="4">
+        <v>3200000</v>
       </c>
       <c r="E71">
         <v>3</v>
       </c>
       <c r="F71" t="s">
-        <v>22</v>
-      </c>
-      <c r="G71" s="5">
-        <v>-9.9999999999999998E+101</v>
+        <v>21</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0</v>
       </c>
       <c r="H71" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2644,51 +2659,51 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>165</v>
+        <v>114</v>
       </c>
       <c r="B72" t="s">
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>166</v>
+        <v>28</v>
       </c>
       <c r="D72">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="E72">
         <v>3</v>
       </c>
       <c r="F72" t="s">
-        <v>22</v>
-      </c>
-      <c r="G72" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H72" s="5">
-        <v>9.9999999999999998E+101</v>
+        <v>23</v>
+      </c>
+      <c r="G72" s="1">
+        <v>0</v>
+      </c>
+      <c r="H72" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="B73" t="s">
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>168</v>
-      </c>
-      <c r="D73">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="D73" s="4">
+        <v>90000</v>
       </c>
       <c r="E73">
         <v>3</v>
       </c>
       <c r="F73" t="s">
-        <v>22</v>
-      </c>
-      <c r="G73" s="5">
-        <v>-9.9999999999999998E+101</v>
+        <v>127</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0</v>
       </c>
       <c r="H73" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2696,16 +2711,16 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>169</v>
+        <v>117</v>
       </c>
       <c r="B74" t="s">
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>170</v>
+        <v>45</v>
       </c>
       <c r="D74">
-        <v>45</v>
+        <v>0.5</v>
       </c>
       <c r="E74">
         <v>3</v>
@@ -2713,8 +2728,8 @@
       <c r="F74" t="s">
         <v>22</v>
       </c>
-      <c r="G74" s="5">
-        <v>-9.9999999999999998E+101</v>
+      <c r="G74" s="1">
+        <v>0</v>
       </c>
       <c r="H74" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2722,13 +2737,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D75">
         <v>45</v>
@@ -2746,9 +2761,61 @@
         <v>9.9999999999999998E+101</v>
       </c>
     </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>142</v>
+      </c>
+      <c r="D76">
+        <v>45</v>
+      </c>
+      <c r="E76">
+        <v>3</v>
+      </c>
+      <c r="F76" t="s">
+        <v>22</v>
+      </c>
+      <c r="G76" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H76" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" t="s">
+        <v>169</v>
+      </c>
+      <c r="C77" t="s">
+        <v>176</v>
+      </c>
+      <c r="D77">
+        <v>100</v>
+      </c>
+      <c r="E77">
+        <v>3</v>
+      </c>
+      <c r="F77" t="s">
+        <v>22</v>
+      </c>
+      <c r="G77" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H77" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H55" xr:uid="{5C6FFFE4-1DCD-43ED-AC49-CFF8C14D347B}">
-    <sortState ref="A2:H55">
+    <sortState ref="A2:H77">
       <sortCondition ref="E1:E55"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
delete inputs , write work around for missing valus
</commit_message>
<xml_diff>
--- a/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
+++ b/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Hotmaps\dispatch_module\cm\app\api_v1\my_calculation_module_directory\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09956563-8E01-4C90-922F-9C62CF728788}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201AEB87-4807-4924-8F2B-BE63702D63AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{A39C18F9-790E-4AC0-B0AE-6D70F2BE89C8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="155">
   <si>
     <t>input_name</t>
   </si>
@@ -204,361 +204,295 @@
     <t>wi_nth</t>
   </si>
   <si>
-    <t>hb_nel</t>
-  </si>
-  <si>
-    <t>hp_nel</t>
-  </si>
-  <si>
-    <t>st_nel</t>
-  </si>
-  <si>
     <t>chp_nel</t>
   </si>
   <si>
+    <t>ir_ir</t>
+  </si>
+  <si>
+    <t>if_if</t>
+  </si>
+  <si>
+    <t>pCO2_pCO2</t>
+  </si>
+  <si>
+    <t>["invest","dispatch"]</t>
+  </si>
+  <si>
+    <t>wood pellets_p</t>
+  </si>
+  <si>
+    <t>bio gas_p</t>
+  </si>
+  <si>
+    <t>['electricity', 'bio gas', 'waste', 'wood pellets', 'radiation', 'various']</t>
+  </si>
+  <si>
+    <t>wood pellets_ef</t>
+  </si>
+  <si>
+    <t>bio gas_ef</t>
+  </si>
+  <si>
+    <t>['bio gas', 'electricity', 'waste', 'wood pellets', 'radiation', 'various']</t>
+  </si>
+  <si>
+    <t>['radiation','electricity', 'bio gas', 'waste', 'wood pellets','various']</t>
+  </si>
+  <si>
+    <t>[ 'wood pellets','electricity', 'bio gas', 'waste', 'radiation', 'various']</t>
+  </si>
+  <si>
+    <t>['waste','electricity', 'bio gas',  'wood pellets', 'radiation', 'various']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy carrier price - Bio Gas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy carrier price - various </t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy carrier price - waste </t>
+  </si>
+  <si>
+    <t xml:space="preserve">electrical efficiency -Back Pressure CHP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy carrier -Back Pressure CHP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lifetime -Back Pressure CHP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEX fix -Back Pressure CHP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEX var -Back Pressure CHP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy carrier -Heat Boiler </t>
+  </si>
+  <si>
+    <t xml:space="preserve">investment cost -Heat Boiler </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lifetime -Heat Boiler </t>
+  </si>
+  <si>
+    <t>emission factor -Bio Gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEX fix -Heat Boiler </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEX var -Heat Boiler </t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy carrier -Heat Pump  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">investment cost -Heat Pump  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lifetime -Heat Pump  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">emission factor -electricity </t>
+  </si>
+  <si>
+    <t>emission factor  -radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEX fix -Heat Pump  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEX var -Heat Pump  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">emission factor  -various </t>
+  </si>
+  <si>
+    <t>energy carrier price -radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy carrier -Solar Thermal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">investment cost -Solar Thermal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lifetime -Solar Thermal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">emission factor  -waste </t>
+  </si>
+  <si>
+    <t xml:space="preserve">emission factor  -wood pellets </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEX fix -Solar Thermal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEX var -Solar Thermal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thermal efficiency -Back Pressure CHP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thermal efficiency -Heat Boiler </t>
+  </si>
+  <si>
+    <t>energy carrier -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t>investment cost -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t>lifetime -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thermal efficiency -Solar Thermal </t>
+  </si>
+  <si>
+    <t>OPEX fix -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t>OPEX var -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t>thermal efficiency -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy carrier price -wood pellets </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Output Capacity  -Back Pressure CHP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">investment cost -Back Pressure CHP </t>
+  </si>
+  <si>
+    <t>invest mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interest rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2 Price </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Output Capacity -Waste Incineration Plant </t>
+  </si>
+  <si>
+    <t>COP -Heat Pump</t>
+  </si>
+  <si>
+    <t>EUR/(MW*yr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity price-Back Pressure CHP </t>
+  </si>
+  <si>
+    <t>electricity price -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t>sale electricity price -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sale electricity price-Back Pressure CHP </t>
+  </si>
+  <si>
+    <t>['hotmaps default hourly profile','fix']</t>
+  </si>
+  <si>
+    <t>chp_elp</t>
+  </si>
+  <si>
+    <t>chp_selp</t>
+  </si>
+  <si>
+    <t>chp_elpSelect</t>
+  </si>
+  <si>
+    <t>chp_selpSelect</t>
+  </si>
+  <si>
+    <t>fix electricity price -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix electricity price-Back Pressure CHP </t>
+  </si>
+  <si>
+    <t>fix sale electricity price -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t>wi_elpSelect</t>
+  </si>
+  <si>
+    <t>wi_selpSelect</t>
+  </si>
+  <si>
+    <t>wi_selp</t>
+  </si>
+  <si>
+    <t>wi_elp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix sale electricity price-Back Pressure CHP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity price -Heat Pump </t>
+  </si>
+  <si>
+    <t>hp_elpSelect</t>
+  </si>
+  <si>
+    <t>hp_elp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity price -Heat Boiler </t>
+  </si>
+  <si>
+    <t>hb_elpSelect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix electricity price -Heat Pump </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix electricity price -Heat Boiler </t>
+  </si>
+  <si>
+    <t>hb_elp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input </t>
+  </si>
+  <si>
+    <t>chp_ramp</t>
+  </si>
+  <si>
+    <t>ramping cost  -Back Pressure CHP</t>
+  </si>
+  <si>
+    <t>ramping cost  -Waste Incineration Plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Output Capacity  -Solar Thermal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Output Capacity  -Heat Pump </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Output Capacity -Heat Boiler </t>
+  </si>
+  <si>
+    <t>wi_ramp</t>
+  </si>
+  <si>
     <t>wi_nel</t>
   </si>
   <si>
-    <t>ir_ir</t>
-  </si>
-  <si>
-    <t>if_if</t>
-  </si>
-  <si>
-    <t>pCO2_pCO2</t>
-  </si>
-  <si>
-    <t>["invest","dispatch"]</t>
-  </si>
-  <si>
-    <t>wood pellets_p</t>
-  </si>
-  <si>
-    <t>bio gas_p</t>
-  </si>
-  <si>
-    <t>['electricity', 'bio gas', 'waste', 'wood pellets', 'radiation', 'various']</t>
-  </si>
-  <si>
-    <t>wood pellets_ef</t>
-  </si>
-  <si>
-    <t>bio gas_ef</t>
-  </si>
-  <si>
-    <t>['bio gas', 'electricity', 'waste', 'wood pellets', 'radiation', 'various']</t>
-  </si>
-  <si>
-    <t>['radiation','electricity', 'bio gas', 'waste', 'wood pellets','various']</t>
-  </si>
-  <si>
-    <t>[ 'wood pellets','electricity', 'bio gas', 'waste', 'radiation', 'various']</t>
-  </si>
-  <si>
-    <t>['waste','electricity', 'bio gas',  'wood pellets', 'radiation', 'various']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">energy carrier price - Bio Gas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">energy carrier price - various </t>
-  </si>
-  <si>
-    <t xml:space="preserve">energy carrier price - waste </t>
-  </si>
-  <si>
-    <t xml:space="preserve">electrical efficiency -Back Pressure CHP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">energy carrier -Back Pressure CHP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lifetime -Back Pressure CHP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">electrical efficiency -Heat Boiler </t>
-  </si>
-  <si>
-    <t>electrical efficiency -Heat Pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEX fix -Back Pressure CHP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEX var -Back Pressure CHP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">electrical efficiency -Solar Thermal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">energy carrier -Heat Boiler </t>
-  </si>
-  <si>
-    <t xml:space="preserve">investment cost -Heat Boiler </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lifetime -Heat Boiler </t>
-  </si>
-  <si>
     <t>electrical efficiency -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t>emission factor -Bio Gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEX fix -Heat Boiler </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEX var -Heat Boiler </t>
-  </si>
-  <si>
-    <t xml:space="preserve">energy carrier -Heat Pump  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">investment cost -Heat Pump  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lifetime -Heat Pump  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">emission factor -electricity </t>
-  </si>
-  <si>
-    <t>emission factor  -radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEX fix -Heat Pump  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEX var -Heat Pump  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">emission factor  -various </t>
-  </si>
-  <si>
-    <t>energy carrier price -radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">energy carrier -Solar Thermal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">investment cost -Solar Thermal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lifetime -Solar Thermal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">emission factor  -waste </t>
-  </si>
-  <si>
-    <t xml:space="preserve">emission factor  -wood pellets </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEX fix -Solar Thermal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEX var -Solar Thermal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">thermal efficiency -Back Pressure CHP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">thermal efficiency -Heat Boiler </t>
-  </si>
-  <si>
-    <t>energy carrier -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t>investment cost -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t>lifetime -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thermal efficiency -Solar Thermal </t>
-  </si>
-  <si>
-    <t>OPEX fix -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t>OPEX var -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t>thermal efficiency -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">energy carrier price -wood pellets </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal Output Capacity  -Back Pressure CHP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">investment cost -Back Pressure CHP </t>
-  </si>
-  <si>
-    <t>invest mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interest rate </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2 Price </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal Output Capacity -Waste Incineration Plant </t>
-  </si>
-  <si>
-    <t>COP -Heat Pump</t>
-  </si>
-  <si>
-    <t>EUR/(MW*yr)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity price-Back Pressure CHP </t>
-  </si>
-  <si>
-    <t>electricity price -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t>sale electricity price -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sale electricity price-Back Pressure CHP </t>
-  </si>
-  <si>
-    <t>['hotmaps default hourly profile','fix']</t>
-  </si>
-  <si>
-    <t>chp_elp</t>
-  </si>
-  <si>
-    <t>chp_selp</t>
-  </si>
-  <si>
-    <t>chp_elpSelect</t>
-  </si>
-  <si>
-    <t>chp_selpSelect</t>
-  </si>
-  <si>
-    <t>fix electricity price -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fix electricity price-Back Pressure CHP </t>
-  </si>
-  <si>
-    <t>fix sale electricity price -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t>wi_elpSelect</t>
-  </si>
-  <si>
-    <t>wi_selpSelect</t>
-  </si>
-  <si>
-    <t>wi_selp</t>
-  </si>
-  <si>
-    <t>wi_elp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fix sale electricity price-Back Pressure CHP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity price -Heat Pump </t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity price -Solar Thermal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sale electricity price -Heat Boiler </t>
-  </si>
-  <si>
-    <t>hp_elpSelect</t>
-  </si>
-  <si>
-    <t>st_elpSelect</t>
-  </si>
-  <si>
-    <t>hb_selpSelect</t>
-  </si>
-  <si>
-    <t>hp_elp</t>
-  </si>
-  <si>
-    <t>st_elp</t>
-  </si>
-  <si>
-    <t>hb_selp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity price -Heat Boiler </t>
-  </si>
-  <si>
-    <t>hb_elpSelect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sale electricity price -Heat Pump </t>
-  </si>
-  <si>
-    <t>hp_selpSelect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sale electricity price -Solar Thermal </t>
-  </si>
-  <si>
-    <t>st_selpSelect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fix electricity price -Heat Pump </t>
-  </si>
-  <si>
-    <t xml:space="preserve">fix electricity price -Solar Thermal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">fix electricity price -Heat Boiler </t>
-  </si>
-  <si>
-    <t>hb_elp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fix sale electricity price -Heat Pump </t>
-  </si>
-  <si>
-    <t>hp_selp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fix sale electricity price -Solar Thermal </t>
-  </si>
-  <si>
-    <t>st_selp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fix sale electricity price -Heat Boiler </t>
-  </si>
-  <si>
-    <t xml:space="preserve">input </t>
-  </si>
-  <si>
-    <t>chp_ramp</t>
-  </si>
-  <si>
-    <t>ramping cost  -Back Pressure CHP</t>
-  </si>
-  <si>
-    <t>ramping cost  -Waste Incineration Plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal Output Capacity  -Solar Thermal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal Output Capacity  -Heat Pump </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal Output Capacity -Heat Boiler </t>
-  </si>
-  <si>
-    <t>wi_ramp</t>
   </si>
 </sst>
 </file>
@@ -929,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED82753-5272-4518-B7D2-E7729D132D1F}">
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +911,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1003,7 +937,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1029,7 +963,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1055,7 +989,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -1081,7 +1015,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -1107,13 +1041,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -1133,13 +1067,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D8">
         <v>7.0000000000000007E-2</v>
@@ -1157,16 +1091,16 @@
     </row>
     <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1176,7 +1110,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -1200,13 +1134,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D11">
         <v>0.2</v>
@@ -1224,16 +1158,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1243,16 +1177,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1262,13 +1196,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D14">
         <v>0.20200000000000001</v>
@@ -1288,7 +1222,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1314,7 +1248,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -1338,16 +1272,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1356,29 +1290,31 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="1">
-        <v>1</v>
+      <c r="H17" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1">
-        <v>0</v>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="5">
+        <v>-9.9999999999999998E+101</v>
       </c>
       <c r="H18" s="5">
         <v>9.9999999999999998E+101</v>
@@ -1386,16 +1322,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1410,13 +1346,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1436,40 +1372,42 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0.114</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <v>1</v>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H21" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1484,160 +1422,162 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>153</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H23" s="5">
-        <v>9.9999999999999998E+101</v>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24">
-        <v>0.114</v>
+        <v>132</v>
+      </c>
+      <c r="D24" t="s">
+        <v>124</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H24" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25">
-        <v>0.6</v>
+        <v>133</v>
+      </c>
+      <c r="D25" t="s">
+        <v>124</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1">
-        <v>1</v>
-      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D26">
-        <v>0.15</v>
+        <v>0.312</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1</v>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H26" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>140</v>
-      </c>
-      <c r="D27" t="s">
-        <v>132</v>
+        <v>64</v>
+      </c>
+      <c r="D27">
+        <v>40</v>
       </c>
       <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H27" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>141</v>
-      </c>
-      <c r="D28" t="s">
-        <v>132</v>
+        <v>48</v>
+      </c>
+      <c r="D28">
+        <v>22</v>
       </c>
       <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H28" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="D29">
-        <v>0.312</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G29" s="5">
         <v>-9.9999999999999998E+101</v>
@@ -1648,16 +1588,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D30">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -1674,16 +1614,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D31">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -1700,19 +1640,19 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" t="s">
         <v>22</v>
@@ -1726,51 +1666,44 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
+        <v>70</v>
       </c>
       <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H33" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="D34" s="4">
+        <v>800000</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" s="5">
-        <v>-9.9999999999999998E+101</v>
+        <v>21</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
       </c>
       <c r="H34" s="5">
         <v>9.9999999999999998E+101</v>
@@ -1778,67 +1711,74 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>169</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>170</v>
+        <v>27</v>
       </c>
       <c r="D35">
+        <v>25</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
         <v>100</v>
-      </c>
-      <c r="E35">
-        <v>3</v>
-      </c>
-      <c r="F35" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H35" s="5">
-        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" t="s">
-        <v>74</v>
+        <v>39</v>
+      </c>
+      <c r="D36" s="4">
+        <v>46000</v>
       </c>
       <c r="E36">
         <v>3</v>
       </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="F36" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="4">
-        <v>800000</v>
+        <v>44</v>
+      </c>
+      <c r="D37">
+        <v>4.5</v>
       </c>
       <c r="E37">
         <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G37" s="1">
         <v>0</v>
@@ -1849,51 +1789,51 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="D38">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E38">
         <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" s="1">
-        <v>0</v>
-      </c>
-      <c r="H38" s="1">
-        <v>100</v>
+        <v>22</v>
+      </c>
+      <c r="G38" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H38" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="4">
-        <v>46000</v>
+        <v>126</v>
+      </c>
+      <c r="D39">
+        <v>45</v>
       </c>
       <c r="E39">
         <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>127</v>
-      </c>
-      <c r="G39" s="1">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="G39" s="5">
+        <v>-9.9999999999999998E+101</v>
       </c>
       <c r="H39" s="5">
         <v>9.9999999999999998E+101</v>
@@ -1901,51 +1841,44 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40">
-        <v>4.5</v>
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
       </c>
       <c r="E40">
         <v>3</v>
       </c>
-      <c r="F40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="1">
-        <v>0</v>
-      </c>
-      <c r="H40" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
-      </c>
-      <c r="D41">
-        <v>45</v>
+        <v>29</v>
+      </c>
+      <c r="D41" s="4">
+        <v>60000</v>
       </c>
       <c r="E41">
         <v>3</v>
       </c>
       <c r="F41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" s="5">
-        <v>-9.9999999999999998E+101</v>
+        <v>21</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
       </c>
       <c r="H41" s="5">
         <v>9.9999999999999998E+101</v>
@@ -1953,67 +1886,74 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>134</v>
+        <v>24</v>
       </c>
       <c r="D42">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E42">
         <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H42" s="5">
-        <v>9.9999999999999998E+101</v>
+        <v>23</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" t="s">
-        <v>72</v>
+        <v>36</v>
+      </c>
+      <c r="D43" s="4">
+        <v>4000</v>
       </c>
       <c r="E43">
         <v>3</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="F43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="4">
-        <v>60000</v>
+        <v>41</v>
+      </c>
+      <c r="D44">
+        <v>1.5</v>
       </c>
       <c r="E44">
         <v>3</v>
       </c>
       <c r="F44" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G44" s="1">
         <v>0</v>
@@ -2024,51 +1964,42 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45">
-        <v>20</v>
+        <v>141</v>
+      </c>
+      <c r="D45" t="s">
+        <v>124</v>
       </c>
       <c r="E45">
         <v>3</v>
-      </c>
-      <c r="F45" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" s="1">
-        <v>0</v>
-      </c>
-      <c r="H45" s="1">
-        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="4">
-        <v>4000</v>
+        <v>144</v>
+      </c>
+      <c r="D46">
+        <v>45</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>127</v>
-      </c>
-      <c r="G46" s="1">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="G46" s="5">
+        <v>-9.9999999999999998E+101</v>
       </c>
       <c r="H46" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2076,85 +2007,87 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D47">
-        <v>1.5</v>
+        <v>138</v>
+      </c>
+      <c r="D47" t="s">
+        <v>124</v>
       </c>
       <c r="E47">
         <v>3</v>
-      </c>
-      <c r="F47" t="s">
-        <v>22</v>
-      </c>
-      <c r="G47" s="1">
-        <v>0</v>
-      </c>
-      <c r="H47" s="5">
-        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>155</v>
-      </c>
-      <c r="D48" t="s">
-        <v>132</v>
+        <v>139</v>
+      </c>
+      <c r="D48">
+        <v>45</v>
       </c>
       <c r="E48">
         <v>3</v>
+      </c>
+      <c r="F48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="5">
+        <v>-9.9999999999999998E+101</v>
+      </c>
+      <c r="H48" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
         <v>20</v>
       </c>
       <c r="C49" t="s">
-        <v>150</v>
+        <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="E49">
         <v>3</v>
       </c>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
-      </c>
-      <c r="D50">
-        <v>45</v>
+        <v>30</v>
+      </c>
+      <c r="D50" s="4">
+        <v>750000</v>
       </c>
       <c r="E50">
         <v>3</v>
       </c>
       <c r="F50" t="s">
-        <v>22</v>
-      </c>
-      <c r="G50" s="5">
-        <v>-9.9999999999999998E+101</v>
+        <v>21</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
       </c>
       <c r="H50" s="5">
         <v>9.9999999999999998E+101</v>
@@ -2162,153 +2095,173 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>168</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="D51">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="E51">
         <v>3</v>
       </c>
       <c r="F51" t="s">
-        <v>22</v>
-      </c>
-      <c r="G51" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H51" s="5">
-        <v>9.9999999999999998E+101</v>
+        <v>23</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
-      </c>
-      <c r="D52" t="s">
-        <v>132</v>
+        <v>37</v>
+      </c>
+      <c r="D52" s="4">
+        <v>34000</v>
       </c>
       <c r="E52">
         <v>3</v>
+      </c>
+      <c r="F52" t="s">
+        <v>119</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>157</v>
-      </c>
-      <c r="D53" t="s">
-        <v>132</v>
+        <v>42</v>
+      </c>
+      <c r="D53">
+        <v>0.5</v>
       </c>
       <c r="E53">
         <v>3</v>
+      </c>
+      <c r="F53" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="5">
+        <v>9.9999999999999998E+101</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C54" t="s">
-        <v>151</v>
-      </c>
-      <c r="D54">
-        <v>45</v>
+        <v>17</v>
+      </c>
+      <c r="D54" t="s">
+        <v>69</v>
       </c>
       <c r="E54">
         <v>3</v>
       </c>
-      <c r="F54" t="s">
-        <v>22</v>
-      </c>
-      <c r="G54" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H54" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>164</v>
+        <v>96</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>165</v>
+        <v>31</v>
       </c>
       <c r="D55">
-        <v>45</v>
+        <v>1030000</v>
       </c>
       <c r="E55">
         <v>3</v>
       </c>
       <c r="F55" t="s">
-        <v>22</v>
-      </c>
-      <c r="G55" s="5">
-        <v>-9.9999999999999998E+101</v>
+        <v>21</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
       </c>
       <c r="H55" s="5">
         <v>9.9999999999999998E+101</v>
       </c>
+      <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56">
         <v>20</v>
       </c>
-      <c r="C56" t="s">
-        <v>16</v>
-      </c>
-      <c r="D56" t="s">
-        <v>69</v>
-      </c>
       <c r="E56">
         <v>3</v>
       </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
+      <c r="F56" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>100</v>
+      </c>
+      <c r="I56" s="1"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D57" s="4">
-        <v>750000</v>
+        <v>30000</v>
       </c>
       <c r="E57">
         <v>3</v>
       </c>
       <c r="F57" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="G57" s="1">
         <v>0</v>
@@ -2316,77 +2269,72 @@
       <c r="H57" s="5">
         <v>9.9999999999999998E+101</v>
       </c>
+      <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D58">
-        <v>25</v>
+        <v>0.5</v>
       </c>
       <c r="E58">
         <v>3</v>
       </c>
       <c r="F58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G58" s="1">
         <v>0</v>
       </c>
-      <c r="H58" s="1">
-        <v>100</v>
-      </c>
+      <c r="H58" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
+      <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
-      </c>
-      <c r="D59" s="4">
-        <v>34000</v>
+        <v>19</v>
+      </c>
+      <c r="D59" t="s">
+        <v>71</v>
       </c>
       <c r="E59">
         <v>3</v>
       </c>
-      <c r="F59" t="s">
-        <v>127</v>
-      </c>
-      <c r="G59" s="1">
-        <v>0</v>
-      </c>
-      <c r="H59" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>42</v>
-      </c>
-      <c r="D60">
-        <v>0.5</v>
+        <v>33</v>
+      </c>
+      <c r="D60" s="4">
+        <v>3200000</v>
       </c>
       <c r="E60">
         <v>3</v>
       </c>
       <c r="F60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G60" s="1">
         <v>0</v>
@@ -2397,41 +2345,48 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" t="s">
-        <v>73</v>
+        <v>28</v>
+      </c>
+      <c r="D61">
+        <v>25</v>
       </c>
       <c r="E61">
         <v>3</v>
       </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
+      <c r="F61" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62">
-        <v>1030000</v>
+        <v>40</v>
+      </c>
+      <c r="D62" s="4">
+        <v>90000</v>
       </c>
       <c r="E62">
         <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="G62" s="1">
         <v>0</v>
@@ -2439,74 +2394,71 @@
       <c r="H62" s="5">
         <v>9.9999999999999998E+101</v>
       </c>
-      <c r="I62" s="1"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D63">
-        <v>20</v>
+        <v>0.5</v>
       </c>
       <c r="E63">
         <v>3</v>
       </c>
       <c r="F63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G63" s="1">
         <v>0</v>
       </c>
-      <c r="H63" s="1">
-        <v>100</v>
-      </c>
-      <c r="I63" s="1"/>
+      <c r="H63" s="5">
+        <v>9.9999999999999998E+101</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>38</v>
-      </c>
-      <c r="D64" s="4">
-        <v>30000</v>
+        <v>135</v>
+      </c>
+      <c r="D64">
+        <v>45</v>
       </c>
       <c r="E64">
         <v>3</v>
       </c>
       <c r="F64" t="s">
-        <v>127</v>
-      </c>
-      <c r="G64" s="1">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="G64" s="5">
+        <v>-9.9999999999999998E+101</v>
       </c>
       <c r="H64" s="5">
         <v>9.9999999999999998E+101</v>
       </c>
-      <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>43</v>
+        <v>134</v>
       </c>
       <c r="D65">
-        <v>0.5</v>
+        <v>45</v>
       </c>
       <c r="E65">
         <v>3</v>
@@ -2514,309 +2466,43 @@
       <c r="F65" t="s">
         <v>22</v>
       </c>
-      <c r="G65" s="1">
-        <v>0</v>
+      <c r="G65" s="5">
+        <v>-9.9999999999999998E+101</v>
       </c>
       <c r="H65" s="5">
         <v>9.9999999999999998E+101</v>
       </c>
-      <c r="I65" s="1"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B66" t="s">
-        <v>20</v>
+        <v>145</v>
       </c>
       <c r="C66" t="s">
-        <v>149</v>
-      </c>
-      <c r="D66" t="s">
-        <v>132</v>
+        <v>152</v>
+      </c>
+      <c r="D66">
+        <v>100</v>
       </c>
       <c r="E66">
         <v>3</v>
       </c>
-      <c r="I66" s="1"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>158</v>
-      </c>
-      <c r="B67" t="s">
-        <v>20</v>
-      </c>
-      <c r="C67" t="s">
-        <v>159</v>
-      </c>
-      <c r="D67" t="s">
-        <v>132</v>
-      </c>
-      <c r="E67">
-        <v>3</v>
-      </c>
-      <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>161</v>
-      </c>
-      <c r="B68" t="s">
-        <v>8</v>
-      </c>
-      <c r="C68" t="s">
-        <v>152</v>
-      </c>
-      <c r="D68">
-        <v>45</v>
-      </c>
-      <c r="E68">
-        <v>3</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="F66" t="s">
         <v>22</v>
       </c>
-      <c r="G68" s="5">
+      <c r="G66" s="5">
         <v>-9.9999999999999998E+101</v>
       </c>
-      <c r="H68" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
-      <c r="I68" s="1"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>166</v>
-      </c>
-      <c r="B69" t="s">
-        <v>8</v>
-      </c>
-      <c r="C69" t="s">
-        <v>167</v>
-      </c>
-      <c r="D69">
-        <v>45</v>
-      </c>
-      <c r="E69">
-        <v>3</v>
-      </c>
-      <c r="F69" t="s">
-        <v>22</v>
-      </c>
-      <c r="G69" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H69" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
-      <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>112</v>
-      </c>
-      <c r="B70" t="s">
-        <v>20</v>
-      </c>
-      <c r="C70" t="s">
-        <v>19</v>
-      </c>
-      <c r="D70" t="s">
-        <v>75</v>
-      </c>
-      <c r="E70">
-        <v>3</v>
-      </c>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>113</v>
-      </c>
-      <c r="B71" t="s">
-        <v>8</v>
-      </c>
-      <c r="C71" t="s">
-        <v>33</v>
-      </c>
-      <c r="D71" s="4">
-        <v>3200000</v>
-      </c>
-      <c r="E71">
-        <v>3</v>
-      </c>
-      <c r="F71" t="s">
-        <v>21</v>
-      </c>
-      <c r="G71" s="1">
-        <v>0</v>
-      </c>
-      <c r="H71" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>114</v>
-      </c>
-      <c r="B72" t="s">
-        <v>8</v>
-      </c>
-      <c r="C72" t="s">
-        <v>28</v>
-      </c>
-      <c r="D72">
-        <v>25</v>
-      </c>
-      <c r="E72">
-        <v>3</v>
-      </c>
-      <c r="F72" t="s">
-        <v>23</v>
-      </c>
-      <c r="G72" s="1">
-        <v>0</v>
-      </c>
-      <c r="H72" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>116</v>
-      </c>
-      <c r="B73" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" t="s">
-        <v>40</v>
-      </c>
-      <c r="D73" s="4">
-        <v>90000</v>
-      </c>
-      <c r="E73">
-        <v>3</v>
-      </c>
-      <c r="F73" t="s">
-        <v>127</v>
-      </c>
-      <c r="G73" s="1">
-        <v>0</v>
-      </c>
-      <c r="H73" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>117</v>
-      </c>
-      <c r="B74" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" t="s">
-        <v>45</v>
-      </c>
-      <c r="D74">
-        <v>0.5</v>
-      </c>
-      <c r="E74">
-        <v>3</v>
-      </c>
-      <c r="F74" t="s">
-        <v>22</v>
-      </c>
-      <c r="G74" s="1">
-        <v>0</v>
-      </c>
-      <c r="H74" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>137</v>
-      </c>
-      <c r="B75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C75" t="s">
-        <v>143</v>
-      </c>
-      <c r="D75">
-        <v>45</v>
-      </c>
-      <c r="E75">
-        <v>3</v>
-      </c>
-      <c r="F75" t="s">
-        <v>22</v>
-      </c>
-      <c r="G75" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H75" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>139</v>
-      </c>
-      <c r="B76" t="s">
-        <v>8</v>
-      </c>
-      <c r="C76" t="s">
-        <v>142</v>
-      </c>
-      <c r="D76">
-        <v>45</v>
-      </c>
-      <c r="E76">
-        <v>3</v>
-      </c>
-      <c r="F76" t="s">
-        <v>22</v>
-      </c>
-      <c r="G76" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H76" s="5">
-        <v>9.9999999999999998E+101</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>172</v>
-      </c>
-      <c r="B77" t="s">
-        <v>169</v>
-      </c>
-      <c r="C77" t="s">
-        <v>176</v>
-      </c>
-      <c r="D77">
-        <v>100</v>
-      </c>
-      <c r="E77">
-        <v>3</v>
-      </c>
-      <c r="F77" t="s">
-        <v>22</v>
-      </c>
-      <c r="G77" s="5">
-        <v>-9.9999999999999998E+101</v>
-      </c>
-      <c r="H77" s="5">
+      <c r="H66" s="5">
         <v>9.9999999999999998E+101</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H55" xr:uid="{5C6FFFE4-1DCD-43ED-AC49-CFF8C14D347B}">
-    <sortState ref="A2:H77">
-      <sortCondition ref="E1:E55"/>
+  <autoFilter ref="A1:H66" xr:uid="{5C6FFFE4-1DCD-43ED-AC49-CFF8C14D347B}">
+    <sortState ref="A2:H66">
+      <sortCondition ref="E1:E48"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bug fix and reorder inputs
reorder delete whithe space for new inputs (ramp)
</commit_message>
<xml_diff>
--- a/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
+++ b/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Hotmaps\dispatch_module\cm\app\api_v1\my_calculation_module_directory\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201AEB87-4807-4924-8F2B-BE63702D63AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E162E66-787D-4D1C-ADD8-CA7D46AE7386}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{A39C18F9-790E-4AC0-B0AE-6D70F2BE89C8}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="154">
   <si>
     <t>input_name</t>
   </si>
@@ -463,9 +463,6 @@
   </si>
   <si>
     <t>hb_elp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">input </t>
   </si>
   <si>
     <t>chp_ramp</t>
@@ -865,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED82753-5272-4518-B7D2-E7729D132D1F}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,7 +934,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -963,7 +960,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -989,7 +986,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -1422,13 +1419,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D23">
         <v>0.2</v>
@@ -1640,13 +1637,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
         <v>145</v>
-      </c>
-      <c r="C32" t="s">
-        <v>146</v>
       </c>
       <c r="D32">
         <v>100</v>
@@ -2475,13 +2472,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B66" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D66">
         <v>100</v>

</xml_diff>

<commit_message>
add new field for district heating demand
</commit_message>
<xml_diff>
--- a/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
+++ b/cm/app/api_v1/my_calculation_module_directory/input_data/INPUTS_CALCULATION_MODULE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20358"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Hotmaps\dispatch_module\cm\app\api_v1\my_calculation_module_directory\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A209B4-2501-42D6-8C99-885D94B0F594}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440F6DA2-F7FD-428E-AA34-B41BC9B1B465}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="1215" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="157">
   <si>
     <t>input_name</t>
   </si>
@@ -482,6 +482,15 @@
   </si>
   <si>
     <t>EUR/(MW*yr)</t>
+  </si>
+  <si>
+    <t>dh_demand</t>
+  </si>
+  <si>
+    <t>MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">district heating demand </t>
   </si>
 </sst>
 </file>
@@ -883,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2485,6 +2494,32 @@
         <v>9.9999999999999998E+101</v>
       </c>
     </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>156</v>
+      </c>
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" t="s">
+        <v>154</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>155</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>9.9999999999999998E+101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>